<commit_message>
1. működő verzió a teljes screenshot megoldással
</commit_message>
<xml_diff>
--- a/prices.xlsx
+++ b/prices.xlsx
@@ -255,7 +255,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="en-HU"/>
           </a:p>
@@ -316,7 +316,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="en-HU"/>
           </a:p>

</xml_diff>